<commit_message>
Plot de las medidas experimentales a la Bitácora
</commit_message>
<xml_diff>
--- a/Codigos de simulación/Datos Experimentales/2025-04-02 Mediciones del perfil.xlsx
+++ b/Codigos de simulación/Datos Experimentales/2025-04-02 Mediciones del perfil.xlsx
@@ -510,7 +510,7 @@
         <v>39.88333333333333</v>
       </c>
       <c r="F3" t="n">
-        <v>0.03333333333333144</v>
+        <v>0.03333333333333381</v>
       </c>
       <c r="G3" t="n">
         <v>22.38333333333333</v>
@@ -533,7 +533,7 @@
         <v>40.37</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0577350269189634</v>
+        <v>0.05773502691896136</v>
       </c>
       <c r="G4" t="n">
         <v>22.87</v>

</xml_diff>